<commit_message>
graficos agora dependendo apenas de invoices
</commit_message>
<xml_diff>
--- a/lib/xlsx_reader/operacoes_em_aberto_biort.xlsx
+++ b/lib/xlsx_reader/operacoes_em_aberto_biort.xlsx
@@ -872,15 +872,6 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -907,6 +898,15 @@
     </xf>
     <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="18" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1264,8 +1264,8 @@
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T24"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="M5" sqref="M5:T24"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1278,15 +1278,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="16" customHeight="1">
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="14"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="24"/>
       <c r="I1" s="9"/>
       <c r="J1" s="9"/>
       <c r="K1" s="9"/>
@@ -1301,64 +1301,64 @@
       <c r="T1" s="10"/>
     </row>
     <row r="2" spans="1:20" ht="21">
-      <c r="A2" s="15">
+      <c r="A2" s="12">
         <v>0</v>
       </c>
-      <c r="B2" s="16">
+      <c r="B2" s="13">
         <v>1</v>
       </c>
-      <c r="C2" s="17">
+      <c r="C2" s="14">
         <v>2</v>
       </c>
-      <c r="D2" s="17">
+      <c r="D2" s="14">
         <v>3</v>
       </c>
-      <c r="E2" s="18">
+      <c r="E2" s="15">
         <v>4</v>
       </c>
-      <c r="F2" s="18">
+      <c r="F2" s="15">
         <v>5</v>
       </c>
-      <c r="G2" s="18">
+      <c r="G2" s="15">
         <v>6</v>
       </c>
-      <c r="H2" s="19">
+      <c r="H2" s="16">
         <v>7</v>
       </c>
-      <c r="I2" s="20">
+      <c r="I2" s="17">
         <v>8</v>
       </c>
-      <c r="J2" s="18">
+      <c r="J2" s="15">
         <v>9</v>
       </c>
-      <c r="K2" s="18">
+      <c r="K2" s="15">
         <v>10</v>
       </c>
-      <c r="L2" s="18">
+      <c r="L2" s="15">
         <v>11</v>
       </c>
-      <c r="M2" s="18">
+      <c r="M2" s="15">
         <v>12</v>
       </c>
-      <c r="N2" s="18">
+      <c r="N2" s="15">
         <v>13</v>
       </c>
-      <c r="O2" s="19">
+      <c r="O2" s="16">
         <v>14</v>
       </c>
-      <c r="P2" s="20">
+      <c r="P2" s="17">
         <v>15</v>
       </c>
-      <c r="Q2" s="18">
+      <c r="Q2" s="15">
         <v>16</v>
       </c>
-      <c r="R2" s="18">
+      <c r="R2" s="15">
         <v>17</v>
       </c>
-      <c r="S2" s="18">
+      <c r="S2" s="15">
         <v>18</v>
       </c>
-      <c r="T2" s="18">
+      <c r="T2" s="15">
         <v>19</v>
       </c>
     </row>
@@ -1372,22 +1372,22 @@
       <c r="D3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="21" t="s">
+      <c r="E3" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="21" t="s">
+      <c r="F3" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="21" t="s">
+      <c r="G3" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="21" t="s">
+      <c r="H3" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="I3" s="21" t="s">
+      <c r="I3" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="J3" s="21" t="s">
+      <c r="J3" s="18" t="s">
         <v>9</v>
       </c>
       <c r="K3" s="2" t="s">
@@ -1429,22 +1429,22 @@
       <c r="D4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E4" s="21" t="s">
+      <c r="E4" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="F4" s="21" t="s">
+      <c r="F4" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="G4" s="21" t="s">
+      <c r="G4" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="H4" s="21" t="s">
+      <c r="H4" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="I4" s="21" t="s">
+      <c r="I4" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="J4" s="21" t="s">
+      <c r="J4" s="18" t="s">
         <v>27</v>
       </c>
       <c r="K4" s="2" t="s">
@@ -1471,52 +1471,52 @@
       <c r="D5" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="E5" s="22" t="s">
+      <c r="E5" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="F5" s="22">
+      <c r="F5" s="19">
         <v>59442.66</v>
       </c>
-      <c r="G5" s="22">
+      <c r="G5" s="19">
         <v>4811.97</v>
       </c>
-      <c r="H5" s="22">
+      <c r="H5" s="19">
         <v>-5.1999999999999998E-2</v>
       </c>
-      <c r="I5" s="22">
+      <c r="I5" s="19">
         <v>136.94999999999999</v>
       </c>
-      <c r="J5" s="22">
+      <c r="J5" s="19">
         <v>-1.5E-3</v>
       </c>
-      <c r="K5" s="22">
+      <c r="K5" s="19">
         <v>46.06</v>
       </c>
-      <c r="L5" s="22">
+      <c r="L5" s="19">
         <v>128.41</v>
       </c>
-      <c r="M5" s="22">
+      <c r="M5" s="19">
         <v>300.74</v>
       </c>
-      <c r="N5" s="22">
+      <c r="N5" s="19">
         <v>0</v>
       </c>
-      <c r="O5" s="22">
+      <c r="O5" s="19">
         <v>54064.59</v>
       </c>
-      <c r="P5" s="22">
+      <c r="P5" s="19">
         <v>0</v>
       </c>
-      <c r="Q5" s="22">
+      <c r="Q5" s="19">
         <v>0</v>
       </c>
-      <c r="R5" s="22">
+      <c r="R5" s="19">
         <v>54064.59</v>
       </c>
-      <c r="S5" s="22">
+      <c r="S5" s="19">
         <v>0</v>
       </c>
-      <c r="T5" s="22">
+      <c r="T5" s="19">
         <v>5077.33</v>
       </c>
     </row>
@@ -1559,13 +1559,13 @@
       <c r="M6" s="6">
         <v>2485</v>
       </c>
-      <c r="N6" s="23"/>
-      <c r="O6" s="23"/>
-      <c r="P6" s="23"/>
-      <c r="Q6" s="23"/>
-      <c r="R6" s="23"/>
-      <c r="S6" s="23"/>
-      <c r="T6" s="24"/>
+      <c r="N6" s="20"/>
+      <c r="O6" s="20"/>
+      <c r="P6" s="20"/>
+      <c r="Q6" s="20"/>
+      <c r="R6" s="20"/>
+      <c r="S6" s="20"/>
+      <c r="T6" s="21"/>
     </row>
     <row r="7" spans="1:20">
       <c r="A7" s="1">
@@ -1606,13 +1606,13 @@
       <c r="M7" s="6">
         <v>18297.66</v>
       </c>
-      <c r="N7" s="23"/>
-      <c r="O7" s="23"/>
-      <c r="P7" s="23"/>
-      <c r="Q7" s="23"/>
-      <c r="R7" s="23"/>
-      <c r="S7" s="23"/>
-      <c r="T7" s="24"/>
+      <c r="N7" s="20"/>
+      <c r="O7" s="20"/>
+      <c r="P7" s="20"/>
+      <c r="Q7" s="20"/>
+      <c r="R7" s="20"/>
+      <c r="S7" s="20"/>
+      <c r="T7" s="21"/>
     </row>
     <row r="8" spans="1:20">
       <c r="A8" s="1">
@@ -1653,13 +1653,13 @@
       <c r="M8" s="6">
         <v>5900</v>
       </c>
-      <c r="N8" s="23"/>
-      <c r="O8" s="23"/>
-      <c r="P8" s="23"/>
-      <c r="Q8" s="23"/>
-      <c r="R8" s="23"/>
-      <c r="S8" s="23"/>
-      <c r="T8" s="24"/>
+      <c r="N8" s="20"/>
+      <c r="O8" s="20"/>
+      <c r="P8" s="20"/>
+      <c r="Q8" s="20"/>
+      <c r="R8" s="20"/>
+      <c r="S8" s="20"/>
+      <c r="T8" s="21"/>
     </row>
     <row r="9" spans="1:20">
       <c r="A9" s="1">
@@ -1700,13 +1700,13 @@
       <c r="M9" s="6">
         <v>4700</v>
       </c>
-      <c r="N9" s="23"/>
-      <c r="O9" s="23"/>
-      <c r="P9" s="23"/>
-      <c r="Q9" s="23"/>
-      <c r="R9" s="23"/>
-      <c r="S9" s="23"/>
-      <c r="T9" s="24"/>
+      <c r="N9" s="20"/>
+      <c r="O9" s="20"/>
+      <c r="P9" s="20"/>
+      <c r="Q9" s="20"/>
+      <c r="R9" s="20"/>
+      <c r="S9" s="20"/>
+      <c r="T9" s="21"/>
     </row>
     <row r="10" spans="1:20">
       <c r="A10" s="1">
@@ -1747,13 +1747,13 @@
       <c r="M10" s="6">
         <v>5900</v>
       </c>
-      <c r="N10" s="23"/>
-      <c r="O10" s="23"/>
-      <c r="P10" s="23"/>
-      <c r="Q10" s="23"/>
-      <c r="R10" s="23"/>
-      <c r="S10" s="23"/>
-      <c r="T10" s="24"/>
+      <c r="N10" s="20"/>
+      <c r="O10" s="20"/>
+      <c r="P10" s="20"/>
+      <c r="Q10" s="20"/>
+      <c r="R10" s="20"/>
+      <c r="S10" s="20"/>
+      <c r="T10" s="21"/>
     </row>
     <row r="11" spans="1:20">
       <c r="A11" s="1">
@@ -1794,13 +1794,13 @@
       <c r="M11" s="6">
         <v>17460</v>
       </c>
-      <c r="N11" s="23"/>
-      <c r="O11" s="23"/>
-      <c r="P11" s="23"/>
-      <c r="Q11" s="23"/>
-      <c r="R11" s="23"/>
-      <c r="S11" s="23"/>
-      <c r="T11" s="24"/>
+      <c r="N11" s="20"/>
+      <c r="O11" s="20"/>
+      <c r="P11" s="20"/>
+      <c r="Q11" s="20"/>
+      <c r="R11" s="20"/>
+      <c r="S11" s="20"/>
+      <c r="T11" s="21"/>
     </row>
     <row r="12" spans="1:20">
       <c r="A12" s="1">
@@ -1841,13 +1841,13 @@
       <c r="M12" s="6">
         <v>4700</v>
       </c>
-      <c r="N12" s="23"/>
-      <c r="O12" s="23"/>
-      <c r="P12" s="23"/>
-      <c r="Q12" s="23"/>
-      <c r="R12" s="23"/>
-      <c r="S12" s="23"/>
-      <c r="T12" s="24"/>
+      <c r="N12" s="20"/>
+      <c r="O12" s="20"/>
+      <c r="P12" s="20"/>
+      <c r="Q12" s="20"/>
+      <c r="R12" s="20"/>
+      <c r="S12" s="20"/>
+      <c r="T12" s="21"/>
     </row>
     <row r="13" spans="1:20">
       <c r="A13" s="1">
@@ -1863,52 +1863,52 @@
       <c r="D13" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="E13" s="22" t="s">
+      <c r="E13" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="F13" s="22">
+      <c r="F13" s="19">
         <v>90974</v>
       </c>
-      <c r="G13" s="22">
+      <c r="G13" s="19">
         <v>6750.49</v>
       </c>
-      <c r="H13" s="22">
+      <c r="H13" s="19">
         <v>-5.1999999999999998E-2</v>
       </c>
-      <c r="I13" s="22">
+      <c r="I13" s="19">
         <v>128.02000000000001</v>
       </c>
-      <c r="J13" s="22">
+      <c r="J13" s="19">
         <v>-1E-3</v>
       </c>
-      <c r="K13" s="22">
+      <c r="K13" s="19">
         <v>42.21</v>
       </c>
-      <c r="L13" s="22">
+      <c r="L13" s="19">
         <v>194.41</v>
       </c>
-      <c r="M13" s="22">
+      <c r="M13" s="19">
         <v>447.34</v>
       </c>
-      <c r="N13" s="22">
+      <c r="N13" s="19">
         <v>0</v>
       </c>
-      <c r="O13" s="22">
+      <c r="O13" s="19">
         <v>83453.740000000005</v>
       </c>
-      <c r="P13" s="22">
+      <c r="P13" s="19">
         <v>0</v>
       </c>
-      <c r="Q13" s="22">
+      <c r="Q13" s="19">
         <v>0</v>
       </c>
-      <c r="R13" s="22">
+      <c r="R13" s="19">
         <v>83453.740000000005</v>
       </c>
-      <c r="S13" s="22">
+      <c r="S13" s="19">
         <v>0</v>
       </c>
-      <c r="T13" s="22">
+      <c r="T13" s="19">
         <v>7072.92</v>
       </c>
     </row>
@@ -1951,13 +1951,13 @@
       <c r="M14" s="6">
         <v>18000</v>
       </c>
-      <c r="N14" s="23"/>
-      <c r="O14" s="23"/>
-      <c r="P14" s="23"/>
-      <c r="Q14" s="23"/>
-      <c r="R14" s="23"/>
-      <c r="S14" s="23"/>
-      <c r="T14" s="24"/>
+      <c r="N14" s="20"/>
+      <c r="O14" s="20"/>
+      <c r="P14" s="20"/>
+      <c r="Q14" s="20"/>
+      <c r="R14" s="20"/>
+      <c r="S14" s="20"/>
+      <c r="T14" s="21"/>
     </row>
     <row r="15" spans="1:20">
       <c r="A15" s="1">
@@ -1998,13 +1998,13 @@
       <c r="M15" s="6">
         <v>6180</v>
       </c>
-      <c r="N15" s="23"/>
-      <c r="O15" s="23"/>
-      <c r="P15" s="23"/>
-      <c r="Q15" s="23"/>
-      <c r="R15" s="23"/>
-      <c r="S15" s="23"/>
-      <c r="T15" s="24"/>
+      <c r="N15" s="20"/>
+      <c r="O15" s="20"/>
+      <c r="P15" s="20"/>
+      <c r="Q15" s="20"/>
+      <c r="R15" s="20"/>
+      <c r="S15" s="20"/>
+      <c r="T15" s="21"/>
     </row>
     <row r="16" spans="1:20">
       <c r="A16" s="1">
@@ -2045,13 +2045,13 @@
       <c r="M16" s="6">
         <v>5200</v>
       </c>
-      <c r="N16" s="23"/>
-      <c r="O16" s="23"/>
-      <c r="P16" s="23"/>
-      <c r="Q16" s="23"/>
-      <c r="R16" s="23"/>
-      <c r="S16" s="23"/>
-      <c r="T16" s="24"/>
+      <c r="N16" s="20"/>
+      <c r="O16" s="20"/>
+      <c r="P16" s="20"/>
+      <c r="Q16" s="20"/>
+      <c r="R16" s="20"/>
+      <c r="S16" s="20"/>
+      <c r="T16" s="21"/>
     </row>
     <row r="17" spans="1:20">
       <c r="A17" s="1">
@@ -2092,13 +2092,13 @@
       <c r="M17" s="6">
         <v>6199</v>
       </c>
-      <c r="N17" s="23"/>
-      <c r="O17" s="23"/>
-      <c r="P17" s="23"/>
-      <c r="Q17" s="23"/>
-      <c r="R17" s="23"/>
-      <c r="S17" s="23"/>
-      <c r="T17" s="24"/>
+      <c r="N17" s="20"/>
+      <c r="O17" s="20"/>
+      <c r="P17" s="20"/>
+      <c r="Q17" s="20"/>
+      <c r="R17" s="20"/>
+      <c r="S17" s="20"/>
+      <c r="T17" s="21"/>
     </row>
     <row r="18" spans="1:20">
       <c r="A18" s="1">
@@ -2139,13 +2139,13 @@
       <c r="M18" s="6">
         <v>10995</v>
       </c>
-      <c r="N18" s="23"/>
-      <c r="O18" s="23"/>
-      <c r="P18" s="23"/>
-      <c r="Q18" s="23"/>
-      <c r="R18" s="23"/>
-      <c r="S18" s="23"/>
-      <c r="T18" s="24"/>
+      <c r="N18" s="20"/>
+      <c r="O18" s="20"/>
+      <c r="P18" s="20"/>
+      <c r="Q18" s="20"/>
+      <c r="R18" s="20"/>
+      <c r="S18" s="20"/>
+      <c r="T18" s="21"/>
     </row>
     <row r="19" spans="1:20">
       <c r="A19" s="1">
@@ -2186,13 +2186,13 @@
       <c r="M19" s="6">
         <v>3800</v>
       </c>
-      <c r="N19" s="23"/>
-      <c r="O19" s="23"/>
-      <c r="P19" s="23"/>
-      <c r="Q19" s="23"/>
-      <c r="R19" s="23"/>
-      <c r="S19" s="23"/>
-      <c r="T19" s="24"/>
+      <c r="N19" s="20"/>
+      <c r="O19" s="20"/>
+      <c r="P19" s="20"/>
+      <c r="Q19" s="20"/>
+      <c r="R19" s="20"/>
+      <c r="S19" s="20"/>
+      <c r="T19" s="21"/>
     </row>
     <row r="20" spans="1:20">
       <c r="A20" s="1">
@@ -2233,13 +2233,13 @@
       <c r="M20" s="6">
         <v>17100</v>
       </c>
-      <c r="N20" s="23"/>
-      <c r="O20" s="23"/>
-      <c r="P20" s="23"/>
-      <c r="Q20" s="23"/>
-      <c r="R20" s="23"/>
-      <c r="S20" s="23"/>
-      <c r="T20" s="24"/>
+      <c r="N20" s="20"/>
+      <c r="O20" s="20"/>
+      <c r="P20" s="20"/>
+      <c r="Q20" s="20"/>
+      <c r="R20" s="20"/>
+      <c r="S20" s="20"/>
+      <c r="T20" s="21"/>
     </row>
     <row r="21" spans="1:20">
       <c r="A21" s="1">
@@ -2280,13 +2280,13 @@
       <c r="M21" s="6">
         <v>7500</v>
       </c>
-      <c r="N21" s="23"/>
-      <c r="O21" s="23"/>
-      <c r="P21" s="23"/>
-      <c r="Q21" s="23"/>
-      <c r="R21" s="23"/>
-      <c r="S21" s="23"/>
-      <c r="T21" s="24"/>
+      <c r="N21" s="20"/>
+      <c r="O21" s="20"/>
+      <c r="P21" s="20"/>
+      <c r="Q21" s="20"/>
+      <c r="R21" s="20"/>
+      <c r="S21" s="20"/>
+      <c r="T21" s="21"/>
     </row>
     <row r="22" spans="1:20">
       <c r="A22" s="1">
@@ -2327,13 +2327,13 @@
       <c r="M22" s="6">
         <v>7000</v>
       </c>
-      <c r="N22" s="23"/>
-      <c r="O22" s="23"/>
-      <c r="P22" s="23"/>
-      <c r="Q22" s="23"/>
-      <c r="R22" s="23"/>
-      <c r="S22" s="23"/>
-      <c r="T22" s="24"/>
+      <c r="N22" s="20"/>
+      <c r="O22" s="20"/>
+      <c r="P22" s="20"/>
+      <c r="Q22" s="20"/>
+      <c r="R22" s="20"/>
+      <c r="S22" s="20"/>
+      <c r="T22" s="21"/>
     </row>
     <row r="23" spans="1:20">
       <c r="A23" s="1">
@@ -2374,13 +2374,13 @@
       <c r="M23" s="6">
         <v>8200</v>
       </c>
-      <c r="N23" s="23"/>
-      <c r="O23" s="23"/>
-      <c r="P23" s="23"/>
-      <c r="Q23" s="23"/>
-      <c r="R23" s="23"/>
-      <c r="S23" s="23"/>
-      <c r="T23" s="24"/>
+      <c r="N23" s="20"/>
+      <c r="O23" s="20"/>
+      <c r="P23" s="20"/>
+      <c r="Q23" s="20"/>
+      <c r="R23" s="20"/>
+      <c r="S23" s="20"/>
+      <c r="T23" s="21"/>
     </row>
     <row r="24" spans="1:20">
       <c r="A24" s="1">
@@ -2421,13 +2421,13 @@
       <c r="M24" s="6">
         <v>800</v>
       </c>
-      <c r="N24" s="23"/>
-      <c r="O24" s="23"/>
-      <c r="P24" s="23"/>
-      <c r="Q24" s="23"/>
-      <c r="R24" s="23"/>
-      <c r="S24" s="23"/>
-      <c r="T24" s="24"/>
+      <c r="N24" s="20"/>
+      <c r="O24" s="20"/>
+      <c r="P24" s="20"/>
+      <c r="Q24" s="20"/>
+      <c r="R24" s="20"/>
+      <c r="S24" s="20"/>
+      <c r="T24" s="21"/>
     </row>
   </sheetData>
   <autoFilter ref="C4:M24"/>

</xml_diff>